<commit_message>
made a htaccess file
</commit_message>
<xml_diff>
--- a/documents2/databasdiagram.xlsx
+++ b/documents2/databasdiagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Dynamiska\OOP_demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\htdocs\dynamiska\Bokhandel2\documents2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6E35981-B8C1-49EC-B06C-432D9DEDE493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBEC126-E826-48CD-BCC9-9E7C82A1FAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A2665FD-8958-4C26-9332-F57E1F3F74F2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A2665FD-8958-4C26-9332-F57E1F3F74F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>table_users</t>
   </si>
@@ -96,6 +96,72 @@
   </si>
   <si>
     <t>INT, 11</t>
+  </si>
+  <si>
+    <t>book_id</t>
+  </si>
+  <si>
+    <t>book_name</t>
+  </si>
+  <si>
+    <t>book_author</t>
+  </si>
+  <si>
+    <t>book_description</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>book_age_rec</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>language_id_fk</t>
+  </si>
+  <si>
+    <t>genre_id_fk</t>
+  </si>
+  <si>
+    <t>book_pages</t>
+  </si>
+  <si>
+    <t>book_price</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> varchar 255</t>
+  </si>
+  <si>
+    <t>book_created</t>
+  </si>
+  <si>
+    <t>book_cover</t>
+  </si>
+  <si>
+    <t>book_featured</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>table_genre</t>
+  </si>
+  <si>
+    <t>genre_id</t>
+  </si>
+  <si>
+    <t>genre_name</t>
+  </si>
+  <si>
+    <t>table_language</t>
+  </si>
+  <si>
+    <t>language_id</t>
+  </si>
+  <si>
+    <t>language_name</t>
   </si>
 </sst>
 </file>
@@ -158,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,7 +306,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>108669</xdr:colOff>
+      <xdr:colOff>41994</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>183894</xdr:rowOff>
     </xdr:to>
@@ -276,6 +342,112 @@
         <a:xfrm rot="12552237">
           <a:off x="3095958" y="1851757"/>
           <a:ext cx="778261" cy="541937"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95068</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>46455</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76645</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Graphic 1" descr="Arrow Right with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC14F4F-CC1E-4CD8-8136-45F15A8C288E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="18214010">
+          <a:off x="5844195" y="3807459"/>
+          <a:ext cx="1121384" cy="560987"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>605925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>160780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>39545</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>143917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Graphic 5" descr="Arrow Right with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC2E61F0-28D3-498B-9E96-CEDBD3C08B13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="12552237">
+          <a:off x="2996700" y="3780280"/>
+          <a:ext cx="1138595" cy="554637"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -584,29 +756,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C96C1C-B07F-410A-8AAC-8520E41B7D96}">
-  <dimension ref="C5:J13"/>
+  <dimension ref="C5:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" customWidth="1"/>
-    <col min="10" max="10" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -614,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
@@ -622,7 +794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="F8" s="2" t="s">
         <v>1</v>
       </c>
@@ -634,11 +806,11 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="F9" s="3" t="s">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -648,15 +820,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -666,41 +838,194 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="F13" s="3" t="s">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>